<commit_message>
Added the request to the OpenStreet API
</commit_message>
<xml_diff>
--- a/src/main/resources/Addresses.xlsx
+++ b/src/main/resources/Addresses.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,38 +20,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">Whitemarsh Ave. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheboygan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wisconsin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gregory Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plainfield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Jersey</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Ruiz de Alarcón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenida Abandoibarra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bilbao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,11 +69,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Nimbus Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,12 +113,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -142,43 +147,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>28014</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>53081</v>
-      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>7060</v>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to write the retrieved data (latitude and longitude) to the Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/Addresses.xlsx
+++ b/src/main/resources/Addresses.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">Ruiz de Alarcón</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madrid</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">San Fernando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sevilla</t>
   </si>
   <si>
     <t xml:space="preserve">España</t>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t xml:space="preserve">48009</t>
+  </si>
+  <si>
+    <t>37.3134419</t>
+  </si>
+  <si>
+    <t>-4.869306</t>
+  </si>
+  <si>
+    <t>43.2687376</t>
+  </si>
+  <si>
+    <t>-2.9404136</t>
   </si>
 </sst>
 </file>
@@ -147,17 +159,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col min="1" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="false" hidden="false" style="1" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -171,10 +183,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>28014</v>
+        <v>41004</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,6 +213,15 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed values moved to a constant value
</commit_message>
<xml_diff>
--- a/src/main/resources/Addresses.xlsx
+++ b/src/main/resources/Addresses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t xml:space="preserve">San Fernando</t>
   </si>
@@ -38,18 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">48009</t>
-  </si>
-  <si>
-    <t>37.3134419</t>
-  </si>
-  <si>
-    <t>-4.869306</t>
-  </si>
-  <si>
-    <t>43.2687376</t>
-  </si>
-  <si>
-    <t>-2.9404136</t>
   </si>
 </sst>
 </file>
@@ -159,17 +147,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="false" hidden="false" style="1" width="11.52" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,12 +176,6 @@
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -210,12 +192,6 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel file data modified
</commit_message>
<xml_diff>
--- a/src/main/resources/Addresses.xlsx
+++ b/src/main/resources/Addresses.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Sevilla</t>
   </si>
   <si>
-    <t xml:space="preserve">España</t>
+    <t xml:space="preserve">Spain</t>
   </si>
   <si>
     <t xml:space="preserve">Avenida Abandoibarra</t>
@@ -150,7 +150,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:I2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>